<commit_message>
incoporate answer by Ron
</commit_message>
<xml_diff>
--- a/compare_cast_reps.xlsx
+++ b/compare_cast_reps.xlsx
@@ -11,7 +11,7 @@
     <sheet name="cast_representations" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">cast_representations!$A$1:$J$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">cast_representations!$A$1:$K$9</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t xml:space="preserve">Order</t>
   </si>
@@ -31,19 +31,22 @@
     <t xml:space="preserve">Cast Representation</t>
   </si>
   <si>
-    <t xml:space="preserve">Proved Correct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Space Eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understandable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementable</t>
+    <t xml:space="preserve">Proved eqv to BC (D)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proved eqv to BC (UD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space-efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blame-tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy to understand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy to implement</t>
   </si>
   <si>
     <t xml:space="preserve">Ind. Compose</t>
@@ -52,46 +55,46 @@
     <t xml:space="preserve">direct def.</t>
   </si>
   <si>
-    <t xml:space="preserve">c ==stx d iff c ==ext d</t>
+    <t xml:space="preserve">c ==stx d iff c ==ext d (D)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c ==stx d iff c ==ext d (UD)</t>
   </si>
   <si>
     <t xml:space="preserve">Types and Labels</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herman's Coercion</t>
   </si>
   <si>
     <t xml:space="preserve">Labeled Coercion</t>
   </si>
   <si>
-    <t xml:space="preserve">Partially UD only</t>
+    <t xml:space="preserve">Partially</t>
   </si>
   <si>
     <t xml:space="preserve">Threesome without Blame</t>
   </si>
   <si>
-    <t xml:space="preserve">UD only</t>
-  </si>
-  <si>
     <t xml:space="preserve">Threesome with Blame</t>
   </si>
   <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
     <t xml:space="preserve">Normal Coercion</t>
   </si>
   <si>
     <t xml:space="preserve">Supercoercion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
   </si>
   <si>
     <t xml:space="preserve">Hyper-coercion</t>
@@ -140,7 +143,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,20 +164,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00A65D"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFED1C24"/>
         <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF58220"/>
-        <bgColor rgb="FFFF6600"/>
+        <fgColor rgb="FF00A65D"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -221,7 +218,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +243,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,23 +255,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,7 +323,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFF58220"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -352,25 +345,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +379,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -401,8 +397,14 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,31 +412,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>12</v>
+      <c r="J2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,31 +450,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,31 +488,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,159 +526,187 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>18</v>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>12</v>
+      <c r="B7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>18</v>
+      <c r="I8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>18</v>
+      <c r="B9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>